<commit_message>
Adeguato test [369] - LDO test case VALIDAZIONE_CDA2_LDO_CT0
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#060000000000XX/INSIEL/CLINICO/G4.3.10/accreditamento-checklist_V8.1.3.xlsx
+++ b/GATEWAY/S1#060000000000XX/INSIEL/CLINICO/G4.3.10/accreditamento-checklist_V8.1.3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://insiel.sharepoint.com/sites/O365-Clinico/Documenti condivisi/PNRR-FSE- Indicatori e  CDA2-Clinico Cardiologia SEI/Clinico/Accreditamento/Documenti da spedire 2023 07 24 G3_4_10/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://insiel.sharepoint.com/sites/O365-Clinico/Documenti condivisi/PNRR-FSE- Indicatori e  CDA2-Clinico Cardiologia SEI/Clinico/Accreditamento/Documenti da spedire 2023 08 03 G4_3_10 Solo Checklist e Data_json/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="437" documentId="8_{FC9E7C34-1270-408E-A0EE-4C2CCF805B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F226CDD4-FCF2-487D-B2D1-D2CBBC3515DF}"/>
+  <xr:revisionPtr revIDLastSave="441" documentId="8_{FC9E7C34-1270-408E-A0EE-4C2CCF805B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD3965AC-4808-4286-9AFF-0856FCAB7D34}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -4587,18 +4587,6 @@
     <t>subject_application_version: G4.3.10</t>
   </si>
   <si>
-    <t>Mon,24 Jul 2023 08:29:50</t>
-  </si>
-  <si>
-    <t>2023-07-24T08:29:50Z</t>
-  </si>
-  <si>
-    <t>497bf70de5ee30e5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.60.4.4.2b1e116a399e50ba22e00d9fc29528b4a33d2e7e44ed83cbf61c99e85bd5f5cf.2e82a3183d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>6574a807401bb12f</t>
   </si>
   <si>
@@ -5094,6 +5082,18 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.60.4.4.07da02a38f6b252723a4f187ef84874ded31b5d669c00431aa4d1976da97abb9.db3071920b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>a977190cf0f95b16</t>
+  </si>
+  <si>
+    <t>Thu,03 Aug 2023 07:38:28</t>
+  </si>
+  <si>
+    <t>2023-08-23T07:38:28Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.60.4.4.2b1e116a399e50ba22e00d9fc29528b4a33d2e7e44ed83cbf61c99e85bd5f5cf.658f484419^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -5513,6 +5513,18 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5534,18 +5546,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8007,10 +8007,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B113" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="G156" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A113" sqref="A113"/>
+      <selection pane="bottomRight" activeCell="I376" sqref="I376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -8049,14 +8049,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38" t="s">
+      <c r="B2" s="41"/>
+      <c r="C2" s="42" t="s">
         <v>850</v>
       </c>
-      <c r="D2" s="37"/>
+      <c r="D2" s="41"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -8074,14 +8074,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="49" t="s">
         <v>849</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="41"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -8099,12 +8099,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="45" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="49" t="s">
         <v>851</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -8123,12 +8123,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="45" t="s">
+      <c r="A5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="49" t="s">
         <v>852</v>
       </c>
-      <c r="D5" s="37"/>
+      <c r="D5" s="41"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -8146,8 +8146,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -8451,16 +8451,16 @@
         <v>59</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>139</v>
@@ -8504,7 +8504,7 @@
         <v>848</v>
       </c>
       <c r="K16" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L16" s="25"/>
       <c r="M16" s="25"/>
@@ -8542,7 +8542,7 @@
         <v>848</v>
       </c>
       <c r="K17" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L17" s="25"/>
       <c r="M17" s="25"/>
@@ -8580,7 +8580,7 @@
         <v>848</v>
       </c>
       <c r="K18" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L18" s="25"/>
       <c r="M18" s="25"/>
@@ -8610,19 +8610,19 @@
       <c r="E19" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="47" t="s">
-        <v>905</v>
-      </c>
-      <c r="G19" s="46" t="s">
-        <v>906</v>
-      </c>
-      <c r="H19" s="46" t="s">
-        <v>904</v>
-      </c>
-      <c r="I19" s="46" t="s">
-        <v>907</v>
-      </c>
-      <c r="J19" s="48" t="s">
+      <c r="F19" s="35" t="s">
+        <v>901</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>902</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>900</v>
+      </c>
+      <c r="I19" s="34" t="s">
+        <v>903</v>
+      </c>
+      <c r="J19" s="36" t="s">
         <v>139</v>
       </c>
       <c r="K19" s="25"/>
@@ -8664,7 +8664,7 @@
         <v>848</v>
       </c>
       <c r="K20" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L20" s="25"/>
       <c r="M20" s="25"/>
@@ -8702,7 +8702,7 @@
         <v>848</v>
       </c>
       <c r="K21" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
@@ -8740,7 +8740,7 @@
         <v>848</v>
       </c>
       <c r="K22" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L22" s="25"/>
       <c r="M22" s="25"/>
@@ -9220,7 +9220,7 @@
         <v>848</v>
       </c>
       <c r="K36" s="25" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="L36" s="25"/>
       <c r="M36" s="25"/>
@@ -9292,7 +9292,7 @@
         <v>848</v>
       </c>
       <c r="K38" s="25" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="L38" s="25"/>
       <c r="M38" s="25"/>
@@ -9330,7 +9330,7 @@
         <v>848</v>
       </c>
       <c r="K39" s="25" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="L39" s="25"/>
       <c r="M39" s="25"/>
@@ -9504,7 +9504,7 @@
         <v>848</v>
       </c>
       <c r="K44" s="25" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="L44" s="25"/>
       <c r="M44" s="25"/>
@@ -9576,7 +9576,7 @@
         <v>848</v>
       </c>
       <c r="K46" s="25" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="L46" s="25"/>
       <c r="M46" s="25"/>
@@ -9614,7 +9614,7 @@
         <v>848</v>
       </c>
       <c r="K47" s="25" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="L47" s="25"/>
       <c r="M47" s="25"/>
@@ -9793,7 +9793,7 @@
       <c r="N52" s="25"/>
       <c r="O52" s="25"/>
       <c r="P52" s="25" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="Q52" s="25"/>
       <c r="R52" s="26" t="s">
@@ -9867,7 +9867,7 @@
       <c r="N54" s="25"/>
       <c r="O54" s="25"/>
       <c r="P54" s="25" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="Q54" s="25"/>
       <c r="R54" s="26" t="s">
@@ -9905,7 +9905,7 @@
       <c r="N55" s="25"/>
       <c r="O55" s="25"/>
       <c r="P55" s="25" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="Q55" s="25"/>
       <c r="R55" s="26" t="s">
@@ -10415,16 +10415,16 @@
         <v>170</v>
       </c>
       <c r="F70" s="23" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="G70" s="24" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="H70" s="24" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="I70" s="24" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="J70" s="25" t="s">
         <v>139</v>
@@ -10437,13 +10437,13 @@
         <v>139</v>
       </c>
       <c r="N70" s="25" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="O70" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P70" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q70" s="25" t="s">
         <v>846</v>
@@ -10471,16 +10471,16 @@
         <v>172</v>
       </c>
       <c r="F71" s="23" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="G71" s="24" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="H71" s="24" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="I71" s="24" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="J71" s="25" t="s">
         <v>139</v>
@@ -10493,13 +10493,13 @@
         <v>139</v>
       </c>
       <c r="N71" s="25" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="O71" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P71" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q71" s="25" t="s">
         <v>846</v>
@@ -10527,16 +10527,16 @@
         <v>174</v>
       </c>
       <c r="F72" s="23" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="H72" s="24" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="I72" s="24" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="J72" s="25" t="s">
         <v>139</v>
@@ -10549,13 +10549,13 @@
         <v>139</v>
       </c>
       <c r="N72" s="25" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="O72" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P72" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q72" s="25" t="s">
         <v>846</v>
@@ -10590,7 +10590,7 @@
         <v>848</v>
       </c>
       <c r="K73" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L73" s="25"/>
       <c r="M73" s="25"/>
@@ -10621,16 +10621,16 @@
         <v>178</v>
       </c>
       <c r="F74" s="23" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="G74" s="24" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="H74" s="24" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="I74" s="24" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="J74" s="25" t="s">
         <v>139</v>
@@ -10643,13 +10643,13 @@
         <v>139</v>
       </c>
       <c r="N74" s="25" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="O74" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P74" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q74" s="25" t="s">
         <v>846</v>
@@ -10677,16 +10677,16 @@
         <v>180</v>
       </c>
       <c r="F75" s="23" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="G75" s="24" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="H75" s="24" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="I75" s="24" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
       <c r="J75" s="25" t="s">
         <v>139</v>
@@ -10699,13 +10699,13 @@
         <v>139</v>
       </c>
       <c r="N75" s="25" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="O75" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P75" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q75" s="25" t="s">
         <v>846</v>
@@ -10733,16 +10733,16 @@
         <v>182</v>
       </c>
       <c r="F76" s="23" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="G76" s="24" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="H76" s="24" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="I76" s="24" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
       <c r="J76" s="25" t="s">
         <v>139</v>
@@ -10755,13 +10755,13 @@
         <v>139</v>
       </c>
       <c r="N76" s="25" t="s">
-        <v>894</v>
+        <v>890</v>
       </c>
       <c r="O76" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P76" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q76" s="25" t="s">
         <v>846</v>
@@ -10789,16 +10789,16 @@
         <v>184</v>
       </c>
       <c r="F77" s="23" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
       <c r="G77" s="24" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
       <c r="H77" s="24" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
       <c r="I77" s="24" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
       <c r="J77" s="25" t="s">
         <v>139</v>
@@ -10811,13 +10811,13 @@
         <v>139</v>
       </c>
       <c r="N77" s="25" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
       <c r="O77" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P77" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q77" s="25" t="s">
         <v>846</v>
@@ -10852,7 +10852,7 @@
         <v>848</v>
       </c>
       <c r="K78" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L78" s="25"/>
       <c r="M78" s="25"/>
@@ -10890,7 +10890,7 @@
         <v>848</v>
       </c>
       <c r="K79" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L79" s="25"/>
       <c r="M79" s="25"/>
@@ -10928,7 +10928,7 @@
         <v>848</v>
       </c>
       <c r="K80" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L80" s="25"/>
       <c r="M80" s="25"/>
@@ -10966,7 +10966,7 @@
         <v>848</v>
       </c>
       <c r="K81" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L81" s="25"/>
       <c r="M81" s="25"/>
@@ -10996,19 +10996,19 @@
       <c r="E82" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="F82" s="47" t="s">
-        <v>908</v>
-      </c>
-      <c r="G82" s="46" t="s">
-        <v>909</v>
-      </c>
-      <c r="H82" s="46" t="s">
-        <v>910</v>
-      </c>
-      <c r="I82" s="46" t="s">
-        <v>911</v>
-      </c>
-      <c r="J82" s="48" t="s">
+      <c r="F82" s="35" t="s">
+        <v>904</v>
+      </c>
+      <c r="G82" s="34" t="s">
+        <v>905</v>
+      </c>
+      <c r="H82" s="34" t="s">
+        <v>906</v>
+      </c>
+      <c r="I82" s="34" t="s">
+        <v>907</v>
+      </c>
+      <c r="J82" s="36" t="s">
         <v>139</v>
       </c>
       <c r="K82" s="25"/>
@@ -11018,14 +11018,14 @@
       <c r="M82" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="N82" s="48" t="s">
-        <v>912</v>
+      <c r="N82" s="36" t="s">
+        <v>908</v>
       </c>
       <c r="O82" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P82" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q82" s="25" t="s">
         <v>846</v>
@@ -11052,17 +11052,17 @@
       <c r="E83" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="F83" s="47" t="s">
-        <v>913</v>
-      </c>
-      <c r="G83" s="46" t="s">
-        <v>914</v>
+      <c r="F83" s="35" t="s">
+        <v>909</v>
+      </c>
+      <c r="G83" s="34" t="s">
+        <v>910</v>
       </c>
       <c r="H83" s="24" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
       <c r="I83" s="24" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="J83" s="25" t="s">
         <v>139</v>
@@ -11075,13 +11075,13 @@
         <v>139</v>
       </c>
       <c r="N83" s="25" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="O83" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P83" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q83" s="25" t="s">
         <v>846</v>
@@ -11108,19 +11108,19 @@
       <c r="E84" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="F84" s="47" t="s">
-        <v>918</v>
-      </c>
-      <c r="G84" s="46" t="s">
-        <v>919</v>
-      </c>
-      <c r="H84" s="46" t="s">
-        <v>916</v>
-      </c>
-      <c r="I84" s="46" t="s">
-        <v>917</v>
-      </c>
-      <c r="J84" s="48" t="s">
+      <c r="F84" s="35" t="s">
+        <v>914</v>
+      </c>
+      <c r="G84" s="34" t="s">
+        <v>915</v>
+      </c>
+      <c r="H84" s="34" t="s">
+        <v>912</v>
+      </c>
+      <c r="I84" s="34" t="s">
+        <v>913</v>
+      </c>
+      <c r="J84" s="36" t="s">
         <v>139</v>
       </c>
       <c r="K84" s="25"/>
@@ -11130,14 +11130,14 @@
       <c r="M84" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="N84" s="48" t="s">
-        <v>920</v>
+      <c r="N84" s="36" t="s">
+        <v>916</v>
       </c>
       <c r="O84" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P84" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q84" s="25" t="s">
         <v>846</v>
@@ -11172,7 +11172,7 @@
         <v>848</v>
       </c>
       <c r="K85" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L85" s="25"/>
       <c r="M85" s="25"/>
@@ -11202,19 +11202,19 @@
       <c r="E86" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="F86" s="47" t="s">
-        <v>921</v>
-      </c>
-      <c r="G86" s="46" t="s">
-        <v>922</v>
-      </c>
-      <c r="H86" s="46" t="s">
-        <v>923</v>
-      </c>
-      <c r="I86" s="46" t="s">
-        <v>924</v>
-      </c>
-      <c r="J86" s="48" t="s">
+      <c r="F86" s="35" t="s">
+        <v>917</v>
+      </c>
+      <c r="G86" s="34" t="s">
+        <v>918</v>
+      </c>
+      <c r="H86" s="34" t="s">
+        <v>919</v>
+      </c>
+      <c r="I86" s="34" t="s">
+        <v>920</v>
+      </c>
+      <c r="J86" s="36" t="s">
         <v>139</v>
       </c>
       <c r="K86" s="25"/>
@@ -11224,14 +11224,14 @@
       <c r="M86" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="N86" s="48" t="s">
-        <v>925</v>
+      <c r="N86" s="36" t="s">
+        <v>921</v>
       </c>
       <c r="O86" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P86" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q86" s="25" t="s">
         <v>846</v>
@@ -11258,19 +11258,19 @@
       <c r="E87" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="F87" s="47" t="s">
-        <v>927</v>
-      </c>
-      <c r="G87" s="46" t="s">
-        <v>928</v>
-      </c>
-      <c r="H87" s="46" t="s">
-        <v>926</v>
-      </c>
-      <c r="I87" s="46" t="s">
-        <v>929</v>
-      </c>
-      <c r="J87" s="48" t="s">
+      <c r="F87" s="35" t="s">
+        <v>923</v>
+      </c>
+      <c r="G87" s="34" t="s">
+        <v>924</v>
+      </c>
+      <c r="H87" s="34" t="s">
+        <v>922</v>
+      </c>
+      <c r="I87" s="34" t="s">
+        <v>925</v>
+      </c>
+      <c r="J87" s="36" t="s">
         <v>139</v>
       </c>
       <c r="K87" s="25"/>
@@ -11280,14 +11280,14 @@
       <c r="M87" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="N87" s="48" t="s">
-        <v>889</v>
+      <c r="N87" s="36" t="s">
+        <v>885</v>
       </c>
       <c r="O87" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P87" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q87" s="25" t="s">
         <v>846</v>
@@ -11314,19 +11314,19 @@
       <c r="E88" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="F88" s="47" t="s">
-        <v>931</v>
-      </c>
-      <c r="G88" s="46" t="s">
-        <v>932</v>
-      </c>
-      <c r="H88" s="46" t="s">
-        <v>930</v>
-      </c>
-      <c r="I88" s="46" t="s">
-        <v>933</v>
-      </c>
-      <c r="J88" s="48" t="s">
+      <c r="F88" s="35" t="s">
+        <v>927</v>
+      </c>
+      <c r="G88" s="34" t="s">
+        <v>928</v>
+      </c>
+      <c r="H88" s="34" t="s">
+        <v>926</v>
+      </c>
+      <c r="I88" s="34" t="s">
+        <v>929</v>
+      </c>
+      <c r="J88" s="36" t="s">
         <v>139</v>
       </c>
       <c r="K88" s="25"/>
@@ -11336,14 +11336,14 @@
       <c r="M88" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="N88" s="48" t="s">
-        <v>934</v>
+      <c r="N88" s="36" t="s">
+        <v>930</v>
       </c>
       <c r="O88" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P88" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q88" s="25" t="s">
         <v>846</v>
@@ -11370,19 +11370,19 @@
       <c r="E89" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="F89" s="47" t="s">
-        <v>936</v>
-      </c>
-      <c r="G89" s="46" t="s">
-        <v>937</v>
-      </c>
-      <c r="H89" s="46" t="s">
-        <v>935</v>
-      </c>
-      <c r="I89" s="46" t="s">
-        <v>938</v>
-      </c>
-      <c r="J89" s="48" t="s">
+      <c r="F89" s="35" t="s">
+        <v>932</v>
+      </c>
+      <c r="G89" s="34" t="s">
+        <v>933</v>
+      </c>
+      <c r="H89" s="34" t="s">
+        <v>931</v>
+      </c>
+      <c r="I89" s="34" t="s">
+        <v>934</v>
+      </c>
+      <c r="J89" s="36" t="s">
         <v>139</v>
       </c>
       <c r="K89" s="25"/>
@@ -11392,14 +11392,14 @@
       <c r="M89" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="N89" s="48" t="s">
-        <v>939</v>
+      <c r="N89" s="36" t="s">
+        <v>935</v>
       </c>
       <c r="O89" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P89" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q89" s="25" t="s">
         <v>846</v>
@@ -11423,22 +11423,22 @@
       <c r="D90" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="E90" s="49" t="s">
+      <c r="E90" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="F90" s="47" t="s">
-        <v>943</v>
-      </c>
-      <c r="G90" s="46" t="s">
-        <v>944</v>
-      </c>
-      <c r="H90" s="46" t="s">
+      <c r="F90" s="35" t="s">
+        <v>939</v>
+      </c>
+      <c r="G90" s="34" t="s">
         <v>940</v>
       </c>
-      <c r="I90" s="46" t="s">
-        <v>942</v>
-      </c>
-      <c r="J90" s="48" t="s">
+      <c r="H90" s="34" t="s">
+        <v>936</v>
+      </c>
+      <c r="I90" s="34" t="s">
+        <v>938</v>
+      </c>
+      <c r="J90" s="36" t="s">
         <v>139</v>
       </c>
       <c r="K90" s="25"/>
@@ -11448,14 +11448,14 @@
       <c r="M90" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="N90" s="48" t="s">
-        <v>941</v>
+      <c r="N90" s="36" t="s">
+        <v>937</v>
       </c>
       <c r="O90" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P90" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q90" s="25" t="s">
         <v>846</v>
@@ -11482,19 +11482,19 @@
       <c r="E91" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="F91" s="47" t="s">
-        <v>947</v>
-      </c>
-      <c r="G91" s="46" t="s">
-        <v>948</v>
-      </c>
-      <c r="H91" s="46" t="s">
+      <c r="F91" s="35" t="s">
+        <v>943</v>
+      </c>
+      <c r="G91" s="34" t="s">
+        <v>944</v>
+      </c>
+      <c r="H91" s="34" t="s">
+        <v>941</v>
+      </c>
+      <c r="I91" s="34" t="s">
         <v>945</v>
       </c>
-      <c r="I91" s="46" t="s">
-        <v>949</v>
-      </c>
-      <c r="J91" s="48" t="s">
+      <c r="J91" s="36" t="s">
         <v>139</v>
       </c>
       <c r="K91" s="25"/>
@@ -11504,14 +11504,14 @@
       <c r="M91" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="N91" s="48" t="s">
-        <v>946</v>
+      <c r="N91" s="36" t="s">
+        <v>942</v>
       </c>
       <c r="O91" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P91" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q91" s="25" t="s">
         <v>846</v>
@@ -11538,19 +11538,19 @@
       <c r="E92" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="F92" s="47" t="s">
-        <v>953</v>
-      </c>
-      <c r="G92" s="46" t="s">
-        <v>954</v>
-      </c>
-      <c r="H92" s="46" t="s">
+      <c r="F92" s="35" t="s">
+        <v>949</v>
+      </c>
+      <c r="G92" s="34" t="s">
         <v>950</v>
       </c>
-      <c r="I92" s="46" t="s">
-        <v>952</v>
-      </c>
-      <c r="J92" s="48" t="s">
+      <c r="H92" s="34" t="s">
+        <v>946</v>
+      </c>
+      <c r="I92" s="34" t="s">
+        <v>948</v>
+      </c>
+      <c r="J92" s="36" t="s">
         <v>139</v>
       </c>
       <c r="K92" s="25"/>
@@ -11560,14 +11560,14 @@
       <c r="M92" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="N92" s="48" t="s">
-        <v>951</v>
+      <c r="N92" s="36" t="s">
+        <v>947</v>
       </c>
       <c r="O92" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P92" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q92" s="25" t="s">
         <v>846</v>
@@ -11602,7 +11602,7 @@
         <v>848</v>
       </c>
       <c r="K93" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L93" s="25"/>
       <c r="M93" s="25"/>
@@ -11640,7 +11640,7 @@
         <v>848</v>
       </c>
       <c r="K94" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L94" s="25"/>
       <c r="M94" s="25"/>
@@ -11678,7 +11678,7 @@
         <v>848</v>
       </c>
       <c r="K95" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L95" s="25"/>
       <c r="M95" s="25"/>
@@ -11716,7 +11716,7 @@
         <v>848</v>
       </c>
       <c r="K96" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L96" s="25"/>
       <c r="M96" s="25"/>
@@ -11754,7 +11754,7 @@
         <v>848</v>
       </c>
       <c r="K97" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L97" s="25"/>
       <c r="M97" s="25"/>
@@ -11792,7 +11792,7 @@
         <v>848</v>
       </c>
       <c r="K98" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L98" s="25"/>
       <c r="M98" s="25"/>
@@ -11830,7 +11830,7 @@
         <v>848</v>
       </c>
       <c r="K99" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L99" s="25"/>
       <c r="M99" s="25"/>
@@ -11868,7 +11868,7 @@
         <v>848</v>
       </c>
       <c r="K100" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L100" s="25"/>
       <c r="M100" s="25"/>
@@ -13700,19 +13700,19 @@
       <c r="E154" s="22" t="s">
         <v>338</v>
       </c>
-      <c r="F154" s="47" t="s">
-        <v>959</v>
-      </c>
-      <c r="G154" s="46" t="s">
-        <v>960</v>
-      </c>
-      <c r="H154" s="46" t="s">
-        <v>961</v>
-      </c>
-      <c r="I154" s="46" t="s">
-        <v>962</v>
-      </c>
-      <c r="J154" s="48" t="s">
+      <c r="F154" s="35" t="s">
+        <v>955</v>
+      </c>
+      <c r="G154" s="34" t="s">
+        <v>956</v>
+      </c>
+      <c r="H154" s="34" t="s">
+        <v>957</v>
+      </c>
+      <c r="I154" s="34" t="s">
+        <v>958</v>
+      </c>
+      <c r="J154" s="36" t="s">
         <v>139</v>
       </c>
       <c r="K154" s="25"/>
@@ -13754,7 +13754,7 @@
         <v>848</v>
       </c>
       <c r="K155" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L155" s="25"/>
       <c r="M155" s="25"/>
@@ -13792,7 +13792,7 @@
         <v>848</v>
       </c>
       <c r="K156" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L156" s="25"/>
       <c r="M156" s="25"/>
@@ -13830,7 +13830,7 @@
         <v>848</v>
       </c>
       <c r="K157" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L157" s="25"/>
       <c r="M157" s="25"/>
@@ -13860,17 +13860,17 @@
       <c r="E158" s="22" t="s">
         <v>346</v>
       </c>
-      <c r="F158" s="47" t="s">
-        <v>964</v>
-      </c>
-      <c r="G158" s="46" t="s">
-        <v>965</v>
+      <c r="F158" s="35" t="s">
+        <v>960</v>
+      </c>
+      <c r="G158" s="34" t="s">
+        <v>961</v>
       </c>
       <c r="H158" s="24" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="I158" s="24" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="J158" s="25" t="s">
         <v>139</v>
@@ -13883,13 +13883,13 @@
         <v>139</v>
       </c>
       <c r="N158" s="25" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
       <c r="O158" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P158" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q158" s="25" t="s">
         <v>846</v>
@@ -13916,17 +13916,17 @@
       <c r="E159" s="22" t="s">
         <v>348</v>
       </c>
-      <c r="F159" s="47" t="s">
-        <v>968</v>
-      </c>
-      <c r="G159" s="46" t="s">
-        <v>969</v>
+      <c r="F159" s="35" t="s">
+        <v>964</v>
+      </c>
+      <c r="G159" s="34" t="s">
+        <v>965</v>
       </c>
       <c r="H159" s="24" t="s">
-        <v>967</v>
+        <v>963</v>
       </c>
       <c r="I159" s="24" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="J159" s="25" t="s">
         <v>139</v>
@@ -13939,13 +13939,13 @@
         <v>139</v>
       </c>
       <c r="N159" s="25" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="O159" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P159" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q159" s="25" t="s">
         <v>846</v>
@@ -13972,17 +13972,17 @@
       <c r="E160" s="22" t="s">
         <v>350</v>
       </c>
-      <c r="F160" s="47" t="s">
-        <v>972</v>
-      </c>
-      <c r="G160" s="46" t="s">
-        <v>973</v>
+      <c r="F160" s="35" t="s">
+        <v>968</v>
+      </c>
+      <c r="G160" s="34" t="s">
+        <v>969</v>
       </c>
       <c r="H160" s="24" t="s">
-        <v>970</v>
+        <v>966</v>
       </c>
       <c r="I160" s="24" t="s">
-        <v>971</v>
+        <v>967</v>
       </c>
       <c r="J160" s="25" t="s">
         <v>139</v>
@@ -13995,13 +13995,13 @@
         <v>139</v>
       </c>
       <c r="N160" s="25" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="O160" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P160" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q160" s="25" t="s">
         <v>846</v>
@@ -14036,7 +14036,7 @@
         <v>848</v>
       </c>
       <c r="K161" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L161" s="25"/>
       <c r="M161" s="25"/>
@@ -14066,17 +14066,17 @@
       <c r="E162" s="22" t="s">
         <v>354</v>
       </c>
-      <c r="F162" s="47" t="s">
-        <v>975</v>
-      </c>
-      <c r="G162" s="46" t="s">
-        <v>976</v>
+      <c r="F162" s="35" t="s">
+        <v>971</v>
+      </c>
+      <c r="G162" s="34" t="s">
+        <v>972</v>
       </c>
       <c r="H162" s="24" t="s">
-        <v>977</v>
+        <v>973</v>
       </c>
       <c r="I162" s="24" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
       <c r="J162" s="25" t="s">
         <v>139</v>
@@ -14089,13 +14089,13 @@
         <v>139</v>
       </c>
       <c r="N162" s="25" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="O162" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P162" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q162" s="25" t="s">
         <v>846</v>
@@ -14122,17 +14122,17 @@
       <c r="E163" s="22" t="s">
         <v>356</v>
       </c>
-      <c r="F163" s="47" t="s">
-        <v>980</v>
-      </c>
-      <c r="G163" s="46" t="s">
-        <v>981</v>
+      <c r="F163" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="G163" s="34" t="s">
+        <v>977</v>
       </c>
       <c r="H163" s="24" t="s">
-        <v>979</v>
+        <v>975</v>
       </c>
       <c r="I163" s="24" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
       <c r="J163" s="25" t="s">
         <v>139</v>
@@ -14145,13 +14145,13 @@
         <v>139</v>
       </c>
       <c r="N163" s="25" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="O163" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P163" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q163" s="25" t="s">
         <v>846</v>
@@ -14186,7 +14186,7 @@
         <v>848</v>
       </c>
       <c r="K164" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L164" s="25"/>
       <c r="M164" s="25"/>
@@ -14216,17 +14216,17 @@
       <c r="E165" s="22" t="s">
         <v>360</v>
       </c>
-      <c r="F165" s="47" t="s">
-        <v>984</v>
-      </c>
-      <c r="G165" s="46" t="s">
-        <v>985</v>
+      <c r="F165" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="G165" s="34" t="s">
+        <v>981</v>
       </c>
       <c r="H165" s="24" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
       <c r="I165" s="24" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
       <c r="J165" s="25" t="s">
         <v>139</v>
@@ -14239,13 +14239,13 @@
         <v>139</v>
       </c>
       <c r="N165" s="25" t="s">
-        <v>987</v>
+        <v>983</v>
       </c>
       <c r="O165" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P165" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q165" s="25" t="s">
         <v>846</v>
@@ -14272,17 +14272,17 @@
       <c r="E166" s="22" t="s">
         <v>362</v>
       </c>
-      <c r="F166" s="47" t="s">
-        <v>991</v>
-      </c>
-      <c r="G166" s="46" t="s">
-        <v>992</v>
+      <c r="F166" s="35" t="s">
+        <v>987</v>
+      </c>
+      <c r="G166" s="34" t="s">
+        <v>988</v>
       </c>
       <c r="H166" s="24" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="I166" s="24" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
       <c r="J166" s="25" t="s">
         <v>139</v>
@@ -14295,13 +14295,13 @@
         <v>139</v>
       </c>
       <c r="N166" s="25" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="O166" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P166" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q166" s="25" t="s">
         <v>846</v>
@@ -14328,17 +14328,17 @@
       <c r="E167" s="22" t="s">
         <v>364</v>
       </c>
-      <c r="F167" s="47" t="s">
-        <v>993</v>
-      </c>
-      <c r="G167" s="46" t="s">
-        <v>994</v>
+      <c r="F167" s="35" t="s">
+        <v>989</v>
+      </c>
+      <c r="G167" s="34" t="s">
+        <v>990</v>
       </c>
       <c r="H167" s="24" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="I167" s="24" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
       <c r="J167" s="25" t="s">
         <v>139</v>
@@ -14351,13 +14351,13 @@
         <v>139</v>
       </c>
       <c r="N167" s="25" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
       <c r="O167" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P167" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q167" s="25" t="s">
         <v>846</v>
@@ -14384,17 +14384,17 @@
       <c r="E168" s="22" t="s">
         <v>366</v>
       </c>
-      <c r="F168" s="47" t="s">
-        <v>1001</v>
-      </c>
-      <c r="G168" s="46" t="s">
-        <v>1002</v>
+      <c r="F168" s="35" t="s">
+        <v>997</v>
+      </c>
+      <c r="G168" s="34" t="s">
+        <v>998</v>
       </c>
       <c r="H168" s="24" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
       <c r="I168" s="24" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
       <c r="J168" s="25" t="s">
         <v>139</v>
@@ -14407,13 +14407,13 @@
         <v>139</v>
       </c>
       <c r="N168" s="25" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
       <c r="O168" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P168" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q168" s="25" t="s">
         <v>846</v>
@@ -14448,7 +14448,7 @@
         <v>848</v>
       </c>
       <c r="K169" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L169" s="25"/>
       <c r="M169" s="25"/>
@@ -14478,17 +14478,17 @@
       <c r="E170" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="F170" s="47" t="s">
-        <v>1007</v>
-      </c>
-      <c r="G170" s="46" t="s">
-        <v>1006</v>
+      <c r="F170" s="35" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G170" s="34" t="s">
+        <v>1002</v>
       </c>
       <c r="H170" s="24" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
       <c r="I170" s="24" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
       <c r="J170" s="25" t="s">
         <v>139</v>
@@ -14501,13 +14501,13 @@
         <v>139</v>
       </c>
       <c r="N170" s="25" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
       <c r="O170" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P170" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q170" s="25" t="s">
         <v>846</v>
@@ -14542,7 +14542,7 @@
         <v>848</v>
       </c>
       <c r="K171" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L171" s="25"/>
       <c r="M171" s="25"/>
@@ -14580,7 +14580,7 @@
         <v>848</v>
       </c>
       <c r="K172" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L172" s="25"/>
       <c r="M172" s="25"/>
@@ -14618,7 +14618,7 @@
         <v>848</v>
       </c>
       <c r="K173" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L173" s="25"/>
       <c r="M173" s="25"/>
@@ -14656,7 +14656,7 @@
         <v>848</v>
       </c>
       <c r="K174" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L174" s="25"/>
       <c r="M174" s="25"/>
@@ -14694,7 +14694,7 @@
         <v>848</v>
       </c>
       <c r="K175" s="25" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="L175" s="25"/>
       <c r="M175" s="25"/>
@@ -14724,17 +14724,17 @@
       <c r="E176" s="22" t="s">
         <v>382</v>
       </c>
-      <c r="F176" s="47" t="s">
-        <v>1011</v>
-      </c>
-      <c r="G176" s="46" t="s">
-        <v>1012</v>
+      <c r="F176" s="35" t="s">
+        <v>1007</v>
+      </c>
+      <c r="G176" s="34" t="s">
+        <v>1008</v>
       </c>
       <c r="H176" s="24" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
       <c r="I176" s="24" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="J176" s="25" t="s">
         <v>139</v>
@@ -14747,13 +14747,13 @@
         <v>139</v>
       </c>
       <c r="N176" s="25" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="O176" s="25" t="s">
         <v>139</v>
       </c>
       <c r="P176" s="25" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="Q176" s="25" t="s">
         <v>846</v>
@@ -21547,16 +21547,16 @@
         <v>780</v>
       </c>
       <c r="F376" s="23" t="s">
-        <v>853</v>
+        <v>1011</v>
       </c>
       <c r="G376" s="24" t="s">
-        <v>854</v>
+        <v>1012</v>
       </c>
       <c r="H376" s="24" t="s">
-        <v>855</v>
+        <v>1010</v>
       </c>
       <c r="I376" s="24" t="s">
-        <v>856</v>
+        <v>1013</v>
       </c>
       <c r="J376" s="25" t="s">
         <v>139</v>
@@ -21592,17 +21592,17 @@
       <c r="E377" s="22" t="s">
         <v>782</v>
       </c>
-      <c r="F377" s="47" t="s">
-        <v>902</v>
-      </c>
-      <c r="G377" s="46" t="s">
-        <v>903</v>
-      </c>
-      <c r="H377" s="46" t="s">
-        <v>900</v>
-      </c>
-      <c r="I377" s="46" t="s">
-        <v>901</v>
+      <c r="F377" s="35" t="s">
+        <v>898</v>
+      </c>
+      <c r="G377" s="34" t="s">
+        <v>899</v>
+      </c>
+      <c r="H377" s="34" t="s">
+        <v>896</v>
+      </c>
+      <c r="I377" s="34" t="s">
+        <v>897</v>
       </c>
       <c r="J377" s="25" t="s">
         <v>139</v>
@@ -21740,19 +21740,19 @@
       <c r="E381" s="22" t="s">
         <v>790</v>
       </c>
-      <c r="F381" s="47" t="s">
-        <v>957</v>
-      </c>
-      <c r="G381" s="46" t="s">
-        <v>958</v>
-      </c>
-      <c r="H381" s="46" t="s">
-        <v>955</v>
-      </c>
-      <c r="I381" s="46" t="s">
-        <v>956</v>
-      </c>
-      <c r="J381" s="48" t="s">
+      <c r="F381" s="35" t="s">
+        <v>953</v>
+      </c>
+      <c r="G381" s="34" t="s">
+        <v>954</v>
+      </c>
+      <c r="H381" s="34" t="s">
+        <v>951</v>
+      </c>
+      <c r="I381" s="34" t="s">
+        <v>952</v>
+      </c>
+      <c r="J381" s="36" t="s">
         <v>139</v>
       </c>
       <c r="K381" s="25"/>
@@ -29259,26 +29259,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ae8219d-8505-4e64-b47a-e5e02bd99ff8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b6c6c545-4433-4453-a388-ae81a1a09069" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BA9DE3DB3C6091468D1D4005047F3381" ma:contentTypeVersion="11" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="cb33f44b3e86db9be098621a95ddc38d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ae8219d-8505-4e64-b47a-e5e02bd99ff8" xmlns:ns3="b6c6c545-4433-4453-a388-ae81a1a09069" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ab53408ccd6a8df5ae8c7fe57b66177a" ns2:_="" ns3:_="">
     <xsd:import namespace="4ae8219d-8505-4e64-b47a-e5e02bd99ff8"/>
@@ -29489,26 +29469,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D90EABD3-6330-4611-9803-3957337B19F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4ae8219d-8505-4e64-b47a-e5e02bd99ff8"/>
-    <ds:schemaRef ds:uri="b6c6c545-4433-4453-a388-ae81a1a09069"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38B9B540-6DAD-4701-9705-A617A590A55F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ae8219d-8505-4e64-b47a-e5e02bd99ff8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b6c6c545-4433-4453-a388-ae81a1a09069" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19ED0497-E7BE-4919-9A94-12345DFDAB70}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -29525,4 +29506,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38B9B540-6DAD-4701-9705-A617A590A55F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D90EABD3-6330-4611-9803-3957337B19F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4ae8219d-8505-4e64-b47a-e5e02bd99ff8"/>
+    <ds:schemaRef ds:uri="b6c6c545-4433-4453-a388-ae81a1a09069"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>